<commit_message>
feat: Implementação da funcionalidade de otimização de carteiras de investimento com PyPortfolioOpt e yfinance.
</commit_message>
<xml_diff>
--- a/src/Analise De Sentimento.xlsx
+++ b/src/Analise De Sentimento.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,37 +446,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ibovespa tem pior ano desde 2021; veja as 10 ações com maiores retornos em 2024</t>
+          <t>Ação do BB (BBAS3) voltou a estar atraente, alerta BTG</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.77</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ibovespa tem pior ano desde 2021; veja as 10 ações com maiores retornos em 2024</t>
+          <t>Estados e municípios contratam R$ 19 bi do BB em crédito com garantia em 2024</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.77</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ibovespa tem pior ano desde 2021; veja as 10 ações com maiores retornos em 2024</t>
+          <t>BB mantém suspensão de consignado do INSS via correspondente</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -485,43 +485,43 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.77</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ibovespa tem pior ano desde 2021; veja as 10 ações com maiores retornos em 2024</t>
+          <t>Dividendos de bancos: Itaú lidera pagamentos em 2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>POSITIVE</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.77</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ibovespa tem pior ano desde 2021; veja as 10 ações com maiores retornos em 2024</t>
+          <t>Banco do Brasil é eleito o mais sustentável do mundo pela sexta vez</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>POSITIVE</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.77</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ibovespa tem pior ano desde 2021; veja as 10 ações com maiores retornos em 2024</t>
+          <t>Ciclo de baixa do Ibovespa está próximo de terminar, diz PagBank</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -530,22 +530,442 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.77</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Suspensão de embarque de soja de 5 empresas para China afeta ações do agro na B3?</t>
+          <t>No Pain, No Gain: Veja 7 ações ‘blindadas’ para períodos ruins</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NEGATIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.84</v>
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ibovespa se livra de crash do DeepSeek e dispara 2%</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ibovespa: Veja os 10 destaques de hoje; Minerva cai mais de 6%</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Ibovespa: Veja os 13 destaques de hoje; Minerva sobe mais de 5%</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ibovespa: Veja os 11 destaques de hoje; Minerva cai mais de 5%</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>UBS BB eleva recomendação de Itaú (ITUB4) para “compra”</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ibovespa: Veja os 13 destaques de hoje; Azul sobe mais de 6%</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ação da Weg (WEGE3) é a que você precisa ter em fevereiro, diz Santander</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BBB1 ao 25: considerando a inflação, qual premiação deu ao ganhador do reality o maior poder de compra?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mesmo em cenário desafiador, é hora de investir, diz estrategista-chefe da XP</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Realização de lucros: o que fez o Ibovespa cair 1,15% após 3 sessões seguidas de alta</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>As ações de dividendos mais indicadas para fevereiro: duas estatais lideram o ranking</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Mesmo elevado, novo teto de juro do consignado do INSS pode ser insuficiente; entenda</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BBA prefere qualidade a valor e rebaixa ação do Bradesco (BBDC4) para neutra</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ETFs de Bitcoin nos EUA completam 1 ano: como foi e o que vem pela frente?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>“Bottom fishing”: Morgan adota estratégia para Brasil e indica ações preferidas</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BB assina termo com BC para devolver R$ 20,6 mi a clientes por cobranças indevidas</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Goldman vê Itaú posicionado para elevar rentabilidade e reforça ação como preferida</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Ibovespa sobe 4,86% em janeiro e tem melhor desempenho desde agosto; alta continuará?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Renda fixa, ações ou internacional? Saiba tudo o que é preciso para investir em 2025</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Ibovespa tem dia de forte ganho com sinais do Copom, apesar de alta de juros; entenda</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Ibovespa volta a superar 127 mil pontos, a caminho de 1ª alta mensal em cinco meses</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Ibovespa fecha em alta, acima dos 126 mil pontos, puxado por Vale e com Itaú em foco</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Por que o Ibovespa sobe cerca de 1% apesar do dia negativo dos mercados globais?</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>O que esperar para bancões? Perspectivas de 2025 mais difícil deve ofuscar bom 4º tri</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Ibovespa: por que dados de inflação dos EUA animam e fazem o índice subir mais de 1%?</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Ao Vivo: Confira os vencedores do Prêmio Outliers InfoMoney</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Temporada de balanços do 4T24 ganha destaque: veja ações e setores para ficar de olho</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>NEUTRAL</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>7 ações sobem mais de 20% e 10 caem mais de 5%: os destaques do Ibovespa em janeiro</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>0.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>